<commit_message>
converting done, finished module testing
</commit_message>
<xml_diff>
--- a/3Final-Project-Test-Cases.xlsx
+++ b/3Final-Project-Test-Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca.sharepoint.com/sites/CPR101_ZII_Thu_130_F23-Bb04/Shared Documents/Bb04/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca-my.sharepoint.com/personal/ldang15_myseneca_ca/Documents/CPRZII/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:1_{FFC6FA63-F955-4637-848C-72668EEFD8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF47441B-5D99-4E10-A06F-7CDC854CD5AE}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="13_ncr:1_{FFC6FA63-F955-4637-848C-72668EEFD8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD2637DA-CB8A-4753-AD77-81F96EAAC134}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
@@ -779,7 +779,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="83">
   <si>
     <t>Program
 or module:</t>
@@ -1139,12 +1139,18 @@
 needs to be submitted.</t>
     </r>
   </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>the program dislays 6 decimal places</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1998,28 +2004,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="e" cm="1">
+      <c r="B1" s="23" t="str" cm="1">
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
-        <v>#VALUE!</v>
+        <v>main</v>
       </c>
       <c r="C1" s="41" t="s">
         <v>1</v>
@@ -2029,7 +2035,7 @@
       <c r="F1" s="42"/>
       <c r="G1" s="42"/>
     </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1">
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
@@ -2044,7 +2050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="26.85" thickBot="1">
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>5</v>
       </c>
@@ -2068,7 +2074,7 @@
       </c>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:9" ht="24">
+    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>12</v>
       </c>
@@ -2095,7 +2101,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="24">
+    <row r="5" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
@@ -2120,7 +2126,7 @@
       <c r="H5" s="25"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="130.5">
+    <row r="6" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
@@ -2145,7 +2151,7 @@
       <c r="H6" s="25"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="24">
+    <row r="7" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
@@ -2173,7 +2179,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="24">
+    <row r="8" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>29</v>
       </c>
@@ -2201,7 +2207,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="24">
+    <row r="9" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>29</v>
       </c>
@@ -2229,7 +2235,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="117">
+    <row r="10" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>29</v>
       </c>
@@ -2257,7 +2263,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="26.1">
+    <row r="11" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>38</v>
       </c>
@@ -2285,7 +2291,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="26.1">
+    <row r="12" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>38</v>
       </c>
@@ -2313,7 +2319,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="51.95">
+    <row r="13" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>38</v>
       </c>
@@ -2341,7 +2347,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="104.1">
+    <row r="14" spans="1:9" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>38</v>
       </c>
@@ -2365,7 +2371,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="39">
+    <row r="15" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>38</v>
       </c>
@@ -2389,7 +2395,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="26.1">
+    <row r="16" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>56</v>
       </c>
@@ -2413,7 +2419,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="26.1">
+    <row r="17" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>56</v>
       </c>
@@ -2441,7 +2447,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="26.1">
+    <row r="18" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>56</v>
       </c>
@@ -2469,7 +2475,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="68.849999999999994" customHeight="1">
+    <row r="19" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>56</v>
       </c>
@@ -2497,7 +2503,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="68.849999999999994" customHeight="1">
+    <row r="20" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
         <v>56</v>
       </c>
@@ -2521,7 +2527,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="68.849999999999994" customHeight="1">
+    <row r="21" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>56</v>
       </c>
@@ -2545,7 +2551,7 @@
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="68.849999999999994" customHeight="1" thickBot="1">
+    <row r="22" spans="1:9" ht="68.849999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
         <v>56</v>
       </c>
@@ -2569,7 +2575,7 @@
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1">
+    <row r="23" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>77</v>
       </c>
@@ -2584,7 +2590,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="26.85" thickBot="1">
+    <row r="24" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
         <v>5</v>
       </c>
@@ -2607,7 +2613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.2">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>12</v>
       </c>
@@ -2621,7 +2627,7 @@
       <c r="G25" s="3"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="15.2">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>12</v>
       </c>
@@ -2635,7 +2641,7 @@
       <c r="G26" s="3"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="15.2">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>12</v>
       </c>
@@ -2649,7 +2655,7 @@
       <c r="G27" s="3"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="15.2">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>29</v>
       </c>
@@ -2663,7 +2669,7 @@
       <c r="G28" s="3"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="15.2">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>29</v>
       </c>
@@ -2677,7 +2683,7 @@
       <c r="G29" s="3"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="15.2">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>29</v>
       </c>
@@ -2691,7 +2697,7 @@
       <c r="G30" s="3"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="15.2">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>38</v>
       </c>
@@ -2705,7 +2711,7 @@
       <c r="G31" s="3"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="15.2">
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>38</v>
       </c>
@@ -2719,7 +2725,7 @@
       <c r="G32" s="3"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="15.2">
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>38</v>
       </c>
@@ -2733,7 +2739,7 @@
       <c r="G33" s="3"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="15.2">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>56</v>
       </c>
@@ -2747,21 +2753,31 @@
       <c r="G34" s="3"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" ht="15.2">
+    <row r="35" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>56</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="3"/>
+      <c r="C35" s="7">
+        <v>1234.123</v>
+      </c>
+      <c r="D35" s="7">
+        <v>1234.123</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1234.123</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="15.95" thickBot="1">
+    <row r="36" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
         <v>56</v>
       </c>
@@ -2775,7 +2791,7 @@
       <c r="G36" s="3"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1">
+    <row r="37" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="39" t="s">
         <v>79</v>
       </c>
@@ -2790,7 +2806,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="26.85" thickBot="1">
+    <row r="38" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="26" t="s">
         <v>5</v>
       </c>
@@ -2813,7 +2829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.2">
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>12</v>
       </c>
@@ -2827,7 +2843,7 @@
       <c r="G39" s="3"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="15.2">
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>12</v>
       </c>
@@ -2841,7 +2857,7 @@
       <c r="G40" s="3"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="15.2">
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>12</v>
       </c>
@@ -2855,7 +2871,7 @@
       <c r="G41" s="3"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="15.2">
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>29</v>
       </c>
@@ -2869,7 +2885,7 @@
       <c r="G42" s="3"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="15.2">
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>29</v>
       </c>
@@ -2883,7 +2899,7 @@
       <c r="G43" s="3"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="15.2">
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>29</v>
       </c>
@@ -2897,7 +2913,7 @@
       <c r="G44" s="3"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="15.2">
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>38</v>
       </c>
@@ -2911,7 +2927,7 @@
       <c r="G45" s="3"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="15.2">
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>38</v>
       </c>
@@ -2925,7 +2941,7 @@
       <c r="G46" s="3"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="15.2">
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>38</v>
       </c>
@@ -2939,7 +2955,7 @@
       <c r="G47" s="3"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="15.2">
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>56</v>
       </c>
@@ -2953,7 +2969,7 @@
       <c r="G48" s="3"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="15.2">
+    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>56</v>
       </c>
@@ -2967,7 +2983,7 @@
       <c r="G49" s="3"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="15.95" thickBot="1">
+    <row r="50" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
         <v>56</v>
       </c>
@@ -2999,12 +3015,12 @@
   <sheetViews>
     <sheetView topLeftCell="AER1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.5703125" customWidth="1"/>
+    <col min="1" max="1" width="89.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="409.5" customHeight="1">
+    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>80</v>
       </c>
@@ -3016,25 +3032,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="834b100a-dc26-4ede-9885-7b3df77c2ec4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041E2C5036B18264388124B3BD1005D20" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b8497cd80e96d74b5b6992e405b57094">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="834b100a-dc26-4ede-9885-7b3df77c2ec4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="059331ad37c3e30d81c2bb785f2f4871" ns2:_="">
     <xsd:import namespace="834b100a-dc26-4ede-9885-7b3df77c2ec4"/>
@@ -3200,14 +3197,57 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="834b100a-dc26-4ede-9885-7b3df77c2ec4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77858E8B-8BDD-41DD-927E-8B417020F918}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D319D43-B1F8-445F-8CD0-0A5D2F76AD13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="834b100a-dc26-4ede-9885-7b3df77c2ec4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDA4F701-CB39-492A-9F08-5608EAF6F285}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDA4F701-CB39-492A-9F08-5608EAF6F285}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D319D43-B1F8-445F-8CD0-0A5D2F76AD13}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77858E8B-8BDD-41DD-927E-8B417020F918}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="834b100a-dc26-4ede-9885-7b3df77c2ec4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
remove .vs and .vscode dir
</commit_message>
<xml_diff>
--- a/3Final-Project-Test-Cases.xlsx
+++ b/3Final-Project-Test-Cases.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cpr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca-my.sharepoint.com/personal/ldang15_myseneca_ca/Documents/CPRZII/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56B7D08-474C-4E75-8674-4E4BE9447635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F56B7D08-474C-4E75-8674-4E4BE9447635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5D1BBC0-9FD7-4914-9C82-13735BE25256}"/>
   <bookViews>
-    <workbookView xWindow="9525" yWindow="0" windowWidth="9750" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
     <sheet name="fundamentals" sheetId="9" r:id="rId2"/>
-    <sheet name="manipulating" sheetId="10" r:id="rId3"/>
-    <sheet name="tokenizing" sheetId="11" r:id="rId4"/>
-    <sheet name="click-drag add module test here" sheetId="8" r:id="rId5"/>
+    <sheet name="converting" sheetId="12" r:id="rId3"/>
+    <sheet name="manipulating" sheetId="10" r:id="rId4"/>
+    <sheet name="tokenizing" sheetId="11" r:id="rId5"/>
+    <sheet name="click-drag add module test here" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1985,7 +1986,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
       <text>
         <r>
           <rPr>
@@ -2029,7 +2030,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
       <text>
         <r>
           <rPr>
@@ -2094,7 +2095,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
       <text>
         <r>
           <rPr>
@@ -2120,7 +2121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
       <text>
         <r>
           <rPr>
@@ -2165,7 +2166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
       <text>
         <r>
           <rPr>
@@ -2189,7 +2190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
       <text>
         <r>
           <rPr>
@@ -2212,7 +2213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
       <text>
         <r>
           <rPr>
@@ -2232,6 +2233,742 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tim McKenna</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{73CDDCC5-DEF9-4198-AB6F-663FBFA75AEC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+general description of a test.
+Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{C5E57DF2-75BE-427E-B461-846D7F195E14}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
++</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{4679AE41-C1FC-42AC-AC68-EBAC777A24D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Test Input:
+exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is similar to source code in a program: it describes exactly how it will be done.
+The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{2891D1DC-16FD-429F-AADE-260368988D34}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output or Response:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+the result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the test is run.
+This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{56C701D0-649D-415A-8827-D8C01E5844B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hover over Result and Comments for more details.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{1CFD9AEA-4F24-48EF-8683-675BA2D08F3F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Result:
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{7AB124D7-8C8A-44DD-A61F-3B2C3D2DE3F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Required for negative test cases that FAIL
+or for unexpect results.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{F73B17DE-5D6D-4BEE-8A16-22F591181658}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+general description of a test.
+Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{F368EADF-F05B-4C15-A4E0-CA9F2F783275}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
++</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{89399E78-2781-46CB-8982-30E3233EC7BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Test Input:
+exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is similar to source code in a program: it describes exactly how it will be done.
+The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{34FB52D3-7A1D-4C5B-9838-1E77E035A0FA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output or Response:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+the result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the test is run.
+This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{400DA026-3EB6-4927-87CA-8598E92E8996}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hover over Result and Comments for more details.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{9E419422-AFBA-4A9D-AF8D-AF50B3D1D5D0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Result:
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{99451D2F-B00E-4B10-92E4-565F887D03DF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Required for negative test cases that FAIL
+or for unexpect results.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+general description of a test.
+Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
++</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Test Input:
+exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is similar to source code in a program: it describes exactly how it will be done.
+The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output or Response:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+the result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the test is run.
+This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hover over Result and Comments for more details.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Result:
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Required for negative test cases that FAIL
+or for unexpect results.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tim McKenna</author>
@@ -2990,7 +3727,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="130">
   <si>
     <t>Program
 or module:</t>
@@ -3482,6 +4219,39 @@
   </si>
   <si>
     <t>,,,,,,,,,,</t>
+  </si>
+  <si>
+    <t>0.000000</t>
+  </si>
+  <si>
+    <t>a warning</t>
+  </si>
+  <si>
+    <t>- unexpected input</t>
+  </si>
+  <si>
+    <t>zasd~</t>
+  </si>
+  <si>
+    <t>The program does not handle strings longer than 16 char correctly</t>
+  </si>
+  <si>
+    <t>11111111111111112.000000</t>
+  </si>
+  <si>
+    <t>11111111111111111</t>
+  </si>
+  <si>
+    <t>- neagetive edge case</t>
+  </si>
+  <si>
+    <t>+ maximum edge case</t>
+  </si>
+  <si>
+    <t>1234.123000</t>
+  </si>
+  <si>
+    <t>Converting</t>
   </si>
 </sst>
 </file>
@@ -3949,7 +4719,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4069,18 +4839,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4095,9 +4853,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4114,12 +4869,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB4B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB4E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4504,22 +5294,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="88" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="88" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.31640625" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.453125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.31640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.31640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.6796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -4527,22 +5317,22 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>main</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="41" t="s">
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
       <c r="F2" s="30" t="s">
         <v>3</v>
       </c>
@@ -4550,7 +5340,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -4574,7 +5364,7 @@
       </c>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>11</v>
       </c>
@@ -4601,7 +5391,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
@@ -4626,7 +5416,7 @@
       <c r="H5" s="25"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="143" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
@@ -4651,7 +5441,7 @@
       <c r="H6" s="25"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="65" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
@@ -4676,7 +5466,7 @@
       <c r="H7" s="25"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
@@ -4704,7 +5494,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="117" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>28</v>
       </c>
@@ -4732,7 +5522,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="117" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>28</v>
       </c>
@@ -4760,7 +5550,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="117" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>28</v>
       </c>
@@ -4788,7 +5578,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -4816,7 +5606,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>37</v>
       </c>
@@ -4844,7 +5634,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="52" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>37</v>
       </c>
@@ -4872,7 +5662,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="39" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>37</v>
       </c>
@@ -4894,7 +5684,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="39" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>37</v>
       </c>
@@ -4918,7 +5708,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>50</v>
       </c>
@@ -4942,7 +5732,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>50</v>
       </c>
@@ -4970,7 +5760,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>50</v>
       </c>
@@ -4998,7 +5788,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="68.900000000000006" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>50</v>
       </c>
@@ -5026,7 +5816,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="68.900000000000006" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>50</v>
       </c>
@@ -5050,7 +5840,7 @@
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="68.900000000000006" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>50</v>
       </c>
@@ -5074,7 +5864,7 @@
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="68.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+    <row r="23" spans="1:9" ht="68.849999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="s">
         <v>50</v>
       </c>
@@ -5098,14 +5888,14 @@
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A24" s="41" t="s">
+    <row r="24" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
       <c r="F24" s="30" t="s">
         <v>3</v>
       </c>
@@ -5113,7 +5903,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
         <v>4</v>
       </c>
@@ -5136,7 +5926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>11</v>
       </c>
@@ -5160,7 +5950,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>11</v>
       </c>
@@ -5184,7 +5974,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>11</v>
       </c>
@@ -5208,7 +5998,7 @@
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>28</v>
       </c>
@@ -5218,7 +6008,7 @@
       <c r="C29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="53" t="s">
+      <c r="D29" s="48" t="s">
         <v>98</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -5232,7 +6022,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>28</v>
       </c>
@@ -5242,7 +6032,7 @@
       <c r="C30" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="53" t="s">
+      <c r="D30" s="48" t="s">
         <v>100</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -5256,7 +6046,7 @@
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="234" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>28</v>
       </c>
@@ -5280,7 +6070,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="65" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>28</v>
       </c>
@@ -5291,7 +6081,7 @@
         <v>103</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="E32" s="54" t="s">
+      <c r="E32" s="49" t="s">
         <v>100</v>
       </c>
       <c r="F32" s="17" t="s">
@@ -5300,7 +6090,7 @@
       <c r="G32" s="3"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="117" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>28</v>
       </c>
@@ -5324,7 +6114,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>37</v>
       </c>
@@ -5346,7 +6136,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>37</v>
       </c>
@@ -5368,7 +6158,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="65" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>37</v>
       </c>
@@ -5390,7 +6180,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="39" x14ac:dyDescent="0.65">
+    <row r="37" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>37</v>
       </c>
@@ -5412,7 +6202,7 @@
       </c>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" ht="15.25" x14ac:dyDescent="0.65">
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>50</v>
       </c>
@@ -5431,7 +6221,7 @@
       </c>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>50</v>
       </c>
@@ -5455,7 +6245,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
         <v>50</v>
       </c>
@@ -5474,14 +6264,14 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A41" s="41" t="s">
+    <row r="41" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
       <c r="F41" s="30" t="s">
         <v>3</v>
       </c>
@@ -5489,7 +6279,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
         <v>4</v>
       </c>
@@ -5512,7 +6302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>11</v>
       </c>
@@ -5526,7 +6316,7 @@
       <c r="G43" s="3"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>11</v>
       </c>
@@ -5540,7 +6330,7 @@
       <c r="G44" s="3"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>11</v>
       </c>
@@ -5554,7 +6344,7 @@
       <c r="G45" s="3"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>28</v>
       </c>
@@ -5568,7 +6358,7 @@
       <c r="G46" s="3"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>28</v>
       </c>
@@ -5582,7 +6372,7 @@
       <c r="G47" s="3"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>28</v>
       </c>
@@ -5596,7 +6386,7 @@
       <c r="G48" s="3"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>37</v>
       </c>
@@ -5610,7 +6400,7 @@
       <c r="G49" s="3"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>37</v>
       </c>
@@ -5624,7 +6414,7 @@
       <c r="G50" s="3"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>37</v>
       </c>
@@ -5638,7 +6428,7 @@
       <c r="G51" s="3"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>50</v>
       </c>
@@ -5652,7 +6442,7 @@
       <c r="G52" s="3"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>50</v>
       </c>
@@ -5666,7 +6456,7 @@
       <c r="G53" s="3"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
         <v>50</v>
       </c>
@@ -5686,36 +6476,36 @@
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="F9:F11">
+    <cfRule type="expression" dxfId="15" priority="3">
+      <formula>ISNUMBER(SEARCH("PASS",$F9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="4">
+      <formula>ISNUMBER(SEARCH("FAIL",$F9))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29:F33">
+    <cfRule type="expression" dxfId="13" priority="1">
+      <formula>ISNUMBER(SEARCH("PASS",$F29))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="2">
+      <formula>ISNUMBER(SEARCH("FAIL",$F29))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F38">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>ISNUMBER(SEARCH("PASS",$F38))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>ISNUMBER(SEARCH("FAIL",$F38))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>ISNUMBER(SEARCH("PASS",$F40))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>ISNUMBER(SEARCH("FAIL",$F40))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9:F11">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>ISNUMBER(SEARCH("PASS",$F9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>ISNUMBER(SEARCH("FAIL",$F9))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F29:F33">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>ISNUMBER(SEARCH("PASS",$F29))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>ISNUMBER(SEARCH("FAIL",$F29))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5732,49 +6522,49 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.40625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="50" t="str">
+      <c r="C1" s="55" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As fundamentals_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="41" t="s">
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="47" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -5793,11 +6583,11 @@
       <c r="F3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>11</v>
       </c>
@@ -5818,7 +6608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
@@ -5839,7 +6629,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="143" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
@@ -5860,7 +6650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="65" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
@@ -5883,7 +6673,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
@@ -5904,31 +6694,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="48"/>
-    </row>
-    <row r="10" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="41" t="s">
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="47" t="s">
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>4</v>
       </c>
@@ -5951,7 +6741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
@@ -5972,7 +6762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -5995,7 +6785,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="208" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="211.2" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>11</v>
       </c>
@@ -6018,7 +6808,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>11</v>
       </c>
@@ -6039,34 +6829,34 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A16" s="46"/>
-      <c r="B16" s="45"/>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="42"/>
+      <c r="B16" s="41"/>
       <c r="E16" s="6"/>
       <c r="F16" s="39"/>
     </row>
-    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A17" s="46"/>
-      <c r="B17" s="45"/>
+    <row r="17" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42"/>
+      <c r="B17" s="41"/>
       <c r="E17" s="6"/>
       <c r="F17" s="39"/>
     </row>
-    <row r="18" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="47" t="s">
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
         <v>4</v>
       </c>
@@ -6089,57 +6879,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A20" s="46"/>
-      <c r="B20" s="45"/>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="41"/>
       <c r="E20" s="6"/>
       <c r="F20" s="39"/>
     </row>
-    <row r="21" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A21" s="46"/>
-      <c r="B21" s="45"/>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="41"/>
       <c r="E21" s="6"/>
       <c r="F21" s="39"/>
     </row>
-    <row r="22" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A22" s="46"/>
-      <c r="B22" s="45"/>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="41"/>
       <c r="E22" s="6"/>
       <c r="F22" s="39"/>
     </row>
-    <row r="23" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A23" s="46"/>
-      <c r="B23" s="45"/>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="41"/>
       <c r="E23" s="6"/>
       <c r="F23" s="39"/>
     </row>
-    <row r="24" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A24" s="46"/>
-      <c r="B24" s="45"/>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="41"/>
       <c r="E24" s="6"/>
       <c r="F24" s="39"/>
     </row>
-    <row r="25" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A25" s="46"/>
-      <c r="B25" s="45"/>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="41"/>
       <c r="E25" s="6"/>
       <c r="F25" s="39"/>
     </row>
-    <row r="26" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A26" s="46"/>
-      <c r="B26" s="45"/>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="41"/>
       <c r="E26" s="6"/>
       <c r="F26" s="39"/>
     </row>
-    <row r="27" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A27" s="46"/>
-      <c r="B27" s="45"/>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="41"/>
       <c r="E27" s="6"/>
       <c r="F27" s="39"/>
     </row>
-    <row r="28" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A28" s="46"/>
-      <c r="B28" s="45"/>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="41"/>
       <c r="E28" s="6"/>
       <c r="F28" s="39"/>
     </row>
@@ -6165,6 +6955,515 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383EB36A-4258-4DB9-A935-1380973574F9}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="55" t="str">
+        <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
+        <v>Save As Converting_test_cases.xlsx</v>
+      </c>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1234.123</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1234.123</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="42"/>
+      <c r="B18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="39"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="42"/>
+      <c r="B19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="39"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="42"/>
+      <c r="B20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="39"/>
+    </row>
+    <row r="21" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="41"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="39"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="41"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="39"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="41"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="39"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="41"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="39"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="41"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="39"/>
+    </row>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="41"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="39"/>
+    </row>
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="42"/>
+      <c r="B29" s="41"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="39"/>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="42"/>
+      <c r="B30" s="41"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="39"/>
+    </row>
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="42"/>
+      <c r="B31" s="41"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="C1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F4:F1048576">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>ISNUMBER(SEARCH("PASS",$F4))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>ISNUMBER(SEARCH("FAIL",$F4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7AA91D-298A-428D-991E-0B5E00F15C05}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -6172,49 +7471,49 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.40625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="50" t="str">
+      <c r="C1" s="55" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As manipulating_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="41" t="s">
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="47" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -6233,11 +7532,11 @@
       <c r="F3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
@@ -6260,7 +7559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>28</v>
       </c>
@@ -6283,7 +7582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="117" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -6306,48 +7605,48 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="33"/>
       <c r="C7" s="34"/>
       <c r="E7" s="34"/>
       <c r="F7" s="39"/>
-      <c r="G7" s="55"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="G7" s="50"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="33"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
       <c r="F8" s="39"/>
-      <c r="G8" s="48"/>
-    </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="G8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="48"/>
-    </row>
-    <row r="10" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="41" t="s">
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="47" t="s">
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>4</v>
       </c>
@@ -6370,7 +7669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>28</v>
       </c>
@@ -6380,7 +7679,7 @@
       <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="48" t="s">
         <v>98</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -6393,7 +7692,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>28</v>
       </c>
@@ -6403,7 +7702,7 @@
       <c r="C13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="48" t="s">
         <v>100</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -6416,7 +7715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="234" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>28</v>
       </c>
@@ -6439,7 +7738,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="65" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>28</v>
       </c>
@@ -6450,7 +7749,7 @@
         <v>103</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="49" t="s">
         <v>100</v>
       </c>
       <c r="F15" s="17" t="s">
@@ -6458,7 +7757,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="117.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:7" ht="119.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>28</v>
       </c>
@@ -6481,22 +7780,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="47" t="s">
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>4</v>
       </c>
@@ -6519,57 +7818,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A19" s="46"/>
-      <c r="B19" s="45"/>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="42"/>
+      <c r="B19" s="41"/>
       <c r="E19" s="6"/>
       <c r="F19" s="39"/>
     </row>
-    <row r="20" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A20" s="46"/>
-      <c r="B20" s="45"/>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="41"/>
       <c r="E20" s="6"/>
       <c r="F20" s="39"/>
     </row>
-    <row r="21" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A21" s="46"/>
-      <c r="B21" s="45"/>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="41"/>
       <c r="E21" s="6"/>
       <c r="F21" s="39"/>
     </row>
-    <row r="22" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A22" s="46"/>
-      <c r="B22" s="45"/>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="41"/>
       <c r="E22" s="6"/>
       <c r="F22" s="39"/>
     </row>
-    <row r="23" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A23" s="46"/>
-      <c r="B23" s="45"/>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="41"/>
       <c r="E23" s="6"/>
       <c r="F23" s="39"/>
     </row>
-    <row r="24" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A24" s="46"/>
-      <c r="B24" s="45"/>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="41"/>
       <c r="E24" s="6"/>
       <c r="F24" s="39"/>
     </row>
-    <row r="25" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A25" s="46"/>
-      <c r="B25" s="45"/>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="41"/>
       <c r="E25" s="6"/>
       <c r="F25" s="39"/>
     </row>
-    <row r="26" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A26" s="46"/>
-      <c r="B26" s="45"/>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="41"/>
       <c r="E26" s="6"/>
       <c r="F26" s="39"/>
     </row>
-    <row r="27" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A27" s="46"/>
-      <c r="B27" s="45"/>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="41"/>
       <c r="E27" s="6"/>
       <c r="F27" s="39"/>
     </row>
@@ -6594,7 +7893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0226E82-A952-4DAE-99A1-1227AB972715}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -6602,49 +7901,49 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.40625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="50" t="str">
+      <c r="C1" s="55" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As fundamentals_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="41" t="s">
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="47" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -6663,11 +7962,11 @@
       <c r="F3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>37</v>
       </c>
@@ -6690,7 +7989,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>37</v>
       </c>
@@ -6713,7 +8012,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="52" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>37</v>
       </c>
@@ -6736,7 +8035,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="39" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>37</v>
       </c>
@@ -6757,7 +8056,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="39" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>37</v>
       </c>
@@ -6780,31 +8079,31 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="48"/>
-    </row>
-    <row r="10" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="41" t="s">
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="47" t="s">
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>4</v>
       </c>
@@ -6827,7 +8126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -6848,7 +8147,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>37</v>
       </c>
@@ -6869,7 +8168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="65" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>37</v>
       </c>
@@ -6890,7 +8189,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="39" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>37</v>
       </c>
@@ -6911,34 +8210,34 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A16" s="46"/>
-      <c r="B16" s="45"/>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="42"/>
+      <c r="B16" s="41"/>
       <c r="E16" s="6"/>
       <c r="F16" s="39"/>
     </row>
-    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A17" s="46"/>
-      <c r="B17" s="45"/>
+    <row r="17" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42"/>
+      <c r="B17" s="41"/>
       <c r="E17" s="6"/>
       <c r="F17" s="39"/>
     </row>
-    <row r="18" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="47" t="s">
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
         <v>4</v>
       </c>
@@ -6961,57 +8260,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A20" s="46"/>
-      <c r="B20" s="45"/>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="41"/>
       <c r="E20" s="6"/>
       <c r="F20" s="39"/>
     </row>
-    <row r="21" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A21" s="46"/>
-      <c r="B21" s="45"/>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="41"/>
       <c r="E21" s="6"/>
       <c r="F21" s="39"/>
     </row>
-    <row r="22" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A22" s="46"/>
-      <c r="B22" s="45"/>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="41"/>
       <c r="E22" s="6"/>
       <c r="F22" s="39"/>
     </row>
-    <row r="23" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A23" s="46"/>
-      <c r="B23" s="45"/>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="41"/>
       <c r="E23" s="6"/>
       <c r="F23" s="39"/>
     </row>
-    <row r="24" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A24" s="46"/>
-      <c r="B24" s="45"/>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="41"/>
       <c r="E24" s="6"/>
       <c r="F24" s="39"/>
     </row>
-    <row r="25" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A25" s="46"/>
-      <c r="B25" s="45"/>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="41"/>
       <c r="E25" s="6"/>
       <c r="F25" s="39"/>
     </row>
-    <row r="26" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A26" s="46"/>
-      <c r="B26" s="45"/>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="41"/>
       <c r="E26" s="6"/>
       <c r="F26" s="39"/>
     </row>
-    <row r="27" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A27" s="46"/>
-      <c r="B27" s="45"/>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="41"/>
       <c r="E27" s="6"/>
       <c r="F27" s="39"/>
     </row>
-    <row r="28" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A28" s="46"/>
-      <c r="B28" s="45"/>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="41"/>
       <c r="E28" s="6"/>
       <c r="F28" s="39"/>
     </row>
@@ -7036,18 +8335,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DE6347-7E0A-47D6-BA4D-B2ACFD9544D5}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="AER1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.54296875" customWidth="1"/>
+    <col min="1" max="1" width="89.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>74</v>
       </c>
@@ -7225,15 +8524,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="834b100a-dc26-4ede-9885-7b3df77c2ec4">
@@ -7241,6 +8531,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7262,14 +8561,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDA4F701-CB39-492A-9F08-5608EAF6F285}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77858E8B-8BDD-41DD-927E-8B417020F918}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7277,4 +8568,12 @@
     <ds:schemaRef ds:uri="834b100a-dc26-4ede-9885-7b3df77c2ec4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDA4F701-CB39-492A-9F08-5608EAF6F285}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ver3: converting.c and converting-git-log.txt is done.
</commit_message>
<xml_diff>
--- a/3Final-Project-Test-Cases.xlsx
+++ b/3Final-Project-Test-Cases.xlsx
@@ -5,20 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca-my.sharepoint.com/personal/ldang15_myseneca_ca/Documents/CPRZII/final_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cpr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F56B7D08-474C-4E75-8674-4E4BE9447635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5D1BBC0-9FD7-4914-9C82-13735BE25256}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56B7D08-474C-4E75-8674-4E4BE9447635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9525" yWindow="0" windowWidth="9750" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
     <sheet name="fundamentals" sheetId="9" r:id="rId2"/>
-    <sheet name="converting" sheetId="12" r:id="rId3"/>
-    <sheet name="manipulating" sheetId="10" r:id="rId4"/>
-    <sheet name="tokenizing" sheetId="11" r:id="rId5"/>
-    <sheet name="click-drag add module test here" sheetId="8" r:id="rId6"/>
+    <sheet name="manipulating" sheetId="10" r:id="rId3"/>
+    <sheet name="tokenizing" sheetId="11" r:id="rId4"/>
+    <sheet name="click-drag add module test here" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1986,7 +1985,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
       <text>
         <r>
           <rPr>
@@ -2030,7 +2029,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
       <text>
         <r>
           <rPr>
@@ -2095,7 +2094,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
+    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
       <text>
         <r>
           <rPr>
@@ -2121,7 +2120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
       <text>
         <r>
           <rPr>
@@ -2166,7 +2165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
       <text>
         <r>
           <rPr>
@@ -2190,7 +2189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
       <text>
         <r>
           <rPr>
@@ -2213,7 +2212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
+    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
       <text>
         <r>
           <rPr>
@@ -2233,742 +2232,6 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Tim McKenna</author>
-  </authors>
-  <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{73CDDCC5-DEF9-4198-AB6F-663FBFA75AEC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-general description of a test.
-Identify the code structure being tested </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">but do not use line numbers – </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>they change</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{C5E57DF2-75BE-427E-B461-846D7F195E14}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-The purpose of the test, also known as Use Case Testing
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-+</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> means a positive test expecting a successful result.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>−</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{4679AE41-C1FC-42AC-AC68-EBAC777A24D9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Test Input:
-exact data for entry to test the purpose.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This is similar to source code in a program: it describes exactly how it will be done.
-The What and Why is in the Description and Purpose.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{2891D1DC-16FD-429F-AADE-260368988D34}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">expected Output or Response:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">reference value to confirm 
-the result – this is documented </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">before </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>the test is run.
-This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{56C701D0-649D-415A-8827-D8C01E5844B0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">…what the heading says. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Hover over Result and Comments for more details.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{1CFD9AEA-4F24-48EF-8683-675BA2D08F3F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Result:
-PASS or FAIL
-+ Positive test cases are expected to PASS.
-- Negative test cases:
-PASS if the program handles input that cannot be processed accurately.
-FAIL if an operating system message appears, or if the program gives inaccurate output. 
-E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
-It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
-It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{7AB124D7-8C8A-44DD-A61F-3B2C3D2DE3F5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Required for negative test cases that FAIL
-or for unexpect results.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{F73B17DE-5D6D-4BEE-8A16-22F591181658}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-general description of a test.
-Identify the code structure being tested </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">but do not use line numbers – </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>they change</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{F368EADF-F05B-4C15-A4E0-CA9F2F783275}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-The purpose of the test, also known as Use Case Testing
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-+</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> means a positive test expecting a successful result.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>−</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{89399E78-2781-46CB-8982-30E3233EC7BC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Test Input:
-exact data for entry to test the purpose.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This is similar to source code in a program: it describes exactly how it will be done.
-The What and Why is in the Description and Purpose.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{34FB52D3-7A1D-4C5B-9838-1E77E035A0FA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">expected Output or Response:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">reference value to confirm 
-the result – this is documented </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">before </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>the test is run.
-This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{400DA026-3EB6-4927-87CA-8598E92E8996}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">…what the heading says. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Hover over Result and Comments for more details.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{9E419422-AFBA-4A9D-AF8D-AF50B3D1D5D0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Result:
-PASS or FAIL
-+ Positive test cases are expected to PASS.
-- Negative test cases:
-PASS if the program handles input that cannot be processed accurately.
-FAIL if an operating system message appears, or if the program gives inaccurate output. 
-E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
-It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
-It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{99451D2F-B00E-4B10-92E4-565F887D03DF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Required for negative test cases that FAIL
-or for unexpect results.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-general description of a test.
-Identify the code structure being tested </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">but do not use line numbers – </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>they change</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-The purpose of the test, also known as Use Case Testing
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-+</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> means a positive test expecting a successful result.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>−</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Test Input:
-exact data for entry to test the purpose.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This is similar to source code in a program: it describes exactly how it will be done.
-The What and Why is in the Description and Purpose.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">expected Output or Response:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">reference value to confirm 
-the result – this is documented </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">before </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>the test is run.
-This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">…what the heading says. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Hover over Result and Comments for more details.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Result:
-PASS or FAIL
-+ Positive test cases are expected to PASS.
-- Negative test cases:
-PASS if the program handles input that cannot be processed accurately.
-FAIL if an operating system message appears, or if the program gives inaccurate output. 
-E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
-It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
-It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Required for negative test cases that FAIL
-or for unexpect results.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tim McKenna</author>
@@ -3727,7 +2990,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="119">
   <si>
     <t>Program
 or module:</t>
@@ -4219,39 +3482,6 @@
   </si>
   <si>
     <t>,,,,,,,,,,</t>
-  </si>
-  <si>
-    <t>0.000000</t>
-  </si>
-  <si>
-    <t>a warning</t>
-  </si>
-  <si>
-    <t>- unexpected input</t>
-  </si>
-  <si>
-    <t>zasd~</t>
-  </si>
-  <si>
-    <t>The program does not handle strings longer than 16 char correctly</t>
-  </si>
-  <si>
-    <t>11111111111111112.000000</t>
-  </si>
-  <si>
-    <t>11111111111111111</t>
-  </si>
-  <si>
-    <t>- neagetive edge case</t>
-  </si>
-  <si>
-    <t>+ maximum edge case</t>
-  </si>
-  <si>
-    <t>1234.123000</t>
-  </si>
-  <si>
-    <t>Converting</t>
   </si>
 </sst>
 </file>
@@ -4719,7 +3949,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4839,6 +4069,18 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4853,6 +4095,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4869,47 +4114,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB4B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -5294,22 +4504,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="88" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="88" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.31640625" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.31640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.31640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.6796875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -5317,22 +4527,22 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>main</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-    </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+    </row>
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
       <c r="F2" s="30" t="s">
         <v>3</v>
       </c>
@@ -5340,7 +4550,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -5364,7 +4574,7 @@
       </c>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.65">
       <c r="A4" s="16" t="s">
         <v>11</v>
       </c>
@@ -5391,7 +4601,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.65">
       <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
@@ -5416,7 +4626,7 @@
       <c r="H5" s="25"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="143" x14ac:dyDescent="0.65">
       <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
@@ -5441,7 +4651,7 @@
       <c r="H6" s="25"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="65" x14ac:dyDescent="0.65">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
@@ -5466,7 +4676,7 @@
       <c r="H7" s="25"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="26" x14ac:dyDescent="0.65">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
@@ -5494,7 +4704,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="117" x14ac:dyDescent="0.6">
       <c r="A9" s="16" t="s">
         <v>28</v>
       </c>
@@ -5522,7 +4732,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="117" x14ac:dyDescent="0.6">
       <c r="A10" s="16" t="s">
         <v>28</v>
       </c>
@@ -5550,7 +4760,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="117" x14ac:dyDescent="0.6">
       <c r="A11" s="16" t="s">
         <v>28</v>
       </c>
@@ -5578,7 +4788,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="26" x14ac:dyDescent="0.6">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -5606,7 +4816,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="26" x14ac:dyDescent="0.6">
       <c r="A13" s="16" t="s">
         <v>37</v>
       </c>
@@ -5634,7 +4844,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="52" x14ac:dyDescent="0.65">
       <c r="A14" s="16" t="s">
         <v>37</v>
       </c>
@@ -5662,7 +4872,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="39" x14ac:dyDescent="0.65">
       <c r="A15" s="16" t="s">
         <v>37</v>
       </c>
@@ -5684,7 +4894,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="39" x14ac:dyDescent="0.65">
       <c r="A16" s="16" t="s">
         <v>37</v>
       </c>
@@ -5708,7 +4918,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="26" x14ac:dyDescent="0.65">
       <c r="A17" s="16" t="s">
         <v>50</v>
       </c>
@@ -5732,7 +4942,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.65">
       <c r="A18" s="16" t="s">
         <v>50</v>
       </c>
@@ -5760,7 +4970,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="26" x14ac:dyDescent="0.65">
       <c r="A19" s="16" t="s">
         <v>50</v>
       </c>
@@ -5788,7 +4998,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="68.900000000000006" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A20" s="16" t="s">
         <v>50</v>
       </c>
@@ -5816,7 +5026,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="68.900000000000006" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A21" s="32" t="s">
         <v>50</v>
       </c>
@@ -5840,7 +5050,7 @@
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="68.900000000000006" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A22" s="32" t="s">
         <v>50</v>
       </c>
@@ -5864,7 +5074,7 @@
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="68.849999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="68.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
       <c r="A23" s="32" t="s">
         <v>50</v>
       </c>
@@ -5888,14 +5098,14 @@
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="51" t="s">
+    <row r="24" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A24" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="30" t="s">
         <v>3</v>
       </c>
@@ -5903,7 +5113,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A25" s="26" t="s">
         <v>4</v>
       </c>
@@ -5926,7 +5136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="26" x14ac:dyDescent="0.65">
       <c r="A26" s="16" t="s">
         <v>11</v>
       </c>
@@ -5950,7 +5160,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.65">
       <c r="A27" s="16" t="s">
         <v>11</v>
       </c>
@@ -5974,7 +5184,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="26" x14ac:dyDescent="0.6">
       <c r="A28" s="16" t="s">
         <v>11</v>
       </c>
@@ -5998,7 +5208,7 @@
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="26" x14ac:dyDescent="0.6">
       <c r="A29" s="16" t="s">
         <v>28</v>
       </c>
@@ -6008,7 +5218,7 @@
       <c r="C29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="48" t="s">
+      <c r="D29" s="53" t="s">
         <v>98</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -6022,7 +5232,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="26" x14ac:dyDescent="0.6">
       <c r="A30" s="16" t="s">
         <v>28</v>
       </c>
@@ -6032,7 +5242,7 @@
       <c r="C30" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="48" t="s">
+      <c r="D30" s="53" t="s">
         <v>100</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -6046,7 +5256,7 @@
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="234" x14ac:dyDescent="0.6">
       <c r="A31" s="16" t="s">
         <v>28</v>
       </c>
@@ -6070,7 +5280,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="65" x14ac:dyDescent="0.6">
       <c r="A32" s="16" t="s">
         <v>28</v>
       </c>
@@ -6081,7 +5291,7 @@
         <v>103</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="54" t="s">
         <v>100</v>
       </c>
       <c r="F32" s="17" t="s">
@@ -6090,7 +5300,7 @@
       <c r="G32" s="3"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="117" x14ac:dyDescent="0.6">
       <c r="A33" s="16" t="s">
         <v>28</v>
       </c>
@@ -6114,7 +5324,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A34" s="16" t="s">
         <v>37</v>
       </c>
@@ -6136,7 +5346,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A35" s="16" t="s">
         <v>37</v>
       </c>
@@ -6158,7 +5368,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="65" x14ac:dyDescent="0.6">
       <c r="A36" s="16" t="s">
         <v>37</v>
       </c>
@@ -6180,7 +5390,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="39" x14ac:dyDescent="0.65">
       <c r="A37" s="16" t="s">
         <v>37</v>
       </c>
@@ -6202,7 +5412,7 @@
       </c>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="15.25" x14ac:dyDescent="0.65">
       <c r="A38" s="16" t="s">
         <v>50</v>
       </c>
@@ -6221,7 +5431,7 @@
       </c>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="26" x14ac:dyDescent="0.6">
       <c r="A39" s="16" t="s">
         <v>50</v>
       </c>
@@ -6245,7 +5455,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A40" s="16" t="s">
         <v>50</v>
       </c>
@@ -6264,14 +5474,14 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="51" t="s">
+    <row r="41" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A41" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="52"/>
-      <c r="C41" s="52"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
       <c r="F41" s="30" t="s">
         <v>3</v>
       </c>
@@ -6279,7 +5489,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A42" s="26" t="s">
         <v>4</v>
       </c>
@@ -6302,7 +5512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A43" s="16" t="s">
         <v>11</v>
       </c>
@@ -6316,7 +5526,7 @@
       <c r="G43" s="3"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A44" s="16" t="s">
         <v>11</v>
       </c>
@@ -6330,7 +5540,7 @@
       <c r="G44" s="3"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A45" s="16" t="s">
         <v>11</v>
       </c>
@@ -6344,7 +5554,7 @@
       <c r="G45" s="3"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A46" s="16" t="s">
         <v>28</v>
       </c>
@@ -6358,7 +5568,7 @@
       <c r="G46" s="3"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A47" s="16" t="s">
         <v>28</v>
       </c>
@@ -6372,7 +5582,7 @@
       <c r="G47" s="3"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A48" s="16" t="s">
         <v>28</v>
       </c>
@@ -6386,7 +5596,7 @@
       <c r="G48" s="3"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A49" s="16" t="s">
         <v>37</v>
       </c>
@@ -6400,7 +5610,7 @@
       <c r="G49" s="3"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A50" s="16" t="s">
         <v>37</v>
       </c>
@@ -6414,7 +5624,7 @@
       <c r="G50" s="3"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A51" s="16" t="s">
         <v>37</v>
       </c>
@@ -6428,7 +5638,7 @@
       <c r="G51" s="3"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A52" s="16" t="s">
         <v>50</v>
       </c>
@@ -6442,7 +5652,7 @@
       <c r="G52" s="3"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A53" s="16" t="s">
         <v>50</v>
       </c>
@@ -6456,7 +5666,7 @@
       <c r="G53" s="3"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A54" s="16" t="s">
         <v>50</v>
       </c>
@@ -6476,36 +5686,36 @@
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="F38">
+    <cfRule type="expression" dxfId="13" priority="7">
+      <formula>ISNUMBER(SEARCH("PASS",$F38))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="8">
+      <formula>ISNUMBER(SEARCH("FAIL",$F38))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40">
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>ISNUMBER(SEARCH("PASS",$F40))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>ISNUMBER(SEARCH("FAIL",$F40))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F9:F11">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>ISNUMBER(SEARCH("PASS",$F9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>ISNUMBER(SEARCH("FAIL",$F9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:F33">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>ISNUMBER(SEARCH("PASS",$F29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>ISNUMBER(SEARCH("FAIL",$F29))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F38">
-    <cfRule type="expression" dxfId="11" priority="7">
-      <formula>ISNUMBER(SEARCH("PASS",$F38))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8">
-      <formula>ISNUMBER(SEARCH("FAIL",$F38))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
-    <cfRule type="expression" dxfId="9" priority="5">
-      <formula>ISNUMBER(SEARCH("PASS",$F40))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
-      <formula>ISNUMBER(SEARCH("FAIL",$F40))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6522,49 +5732,49 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.40625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="55" t="str">
+      <c r="C1" s="50" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As fundamentals_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-    </row>
-    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+    </row>
+    <row r="2" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="43" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="47" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -6583,11 +5793,11 @@
       <c r="F3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A4" s="16" t="s">
         <v>11</v>
       </c>
@@ -6608,7 +5818,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
@@ -6629,7 +5839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="143" x14ac:dyDescent="0.6">
       <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
@@ -6650,7 +5860,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="65" x14ac:dyDescent="0.6">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
@@ -6673,7 +5883,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
@@ -6694,31 +5904,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A9" s="34"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="44"/>
-    </row>
-    <row r="10" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51" t="s">
+      <c r="G9" s="48"/>
+    </row>
+    <row r="10" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A10" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="43" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="47" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A11" s="26" t="s">
         <v>4</v>
       </c>
@@ -6741,7 +5951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
@@ -6762,7 +5972,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -6785,7 +5995,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="211.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="208" x14ac:dyDescent="0.6">
       <c r="A14" s="16" t="s">
         <v>11</v>
       </c>
@@ -6808,7 +6018,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A15" s="16" t="s">
         <v>11</v>
       </c>
@@ -6829,34 +6039,34 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
-      <c r="B16" s="41"/>
+    <row r="16" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A16" s="46"/>
+      <c r="B16" s="45"/>
       <c r="E16" s="6"/>
       <c r="F16" s="39"/>
     </row>
-    <row r="17" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
-      <c r="B17" s="41"/>
+    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A17" s="46"/>
+      <c r="B17" s="45"/>
       <c r="E17" s="6"/>
       <c r="F17" s="39"/>
     </row>
-    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51" t="s">
+    <row r="18" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A18" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="43" t="s">
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="47" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A19" s="26" t="s">
         <v>4</v>
       </c>
@@ -6879,57 +6089,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
-      <c r="B20" s="41"/>
+    <row r="20" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A20" s="46"/>
+      <c r="B20" s="45"/>
       <c r="E20" s="6"/>
       <c r="F20" s="39"/>
     </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="41"/>
+    <row r="21" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A21" s="46"/>
+      <c r="B21" s="45"/>
       <c r="E21" s="6"/>
       <c r="F21" s="39"/>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="41"/>
+    <row r="22" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A22" s="46"/>
+      <c r="B22" s="45"/>
       <c r="E22" s="6"/>
       <c r="F22" s="39"/>
     </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="41"/>
+    <row r="23" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A23" s="46"/>
+      <c r="B23" s="45"/>
       <c r="E23" s="6"/>
       <c r="F23" s="39"/>
     </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="41"/>
+    <row r="24" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A24" s="46"/>
+      <c r="B24" s="45"/>
       <c r="E24" s="6"/>
       <c r="F24" s="39"/>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="41"/>
+    <row r="25" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A25" s="46"/>
+      <c r="B25" s="45"/>
       <c r="E25" s="6"/>
       <c r="F25" s="39"/>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="41"/>
+    <row r="26" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A26" s="46"/>
+      <c r="B26" s="45"/>
       <c r="E26" s="6"/>
       <c r="F26" s="39"/>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="41"/>
+    <row r="27" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A27" s="46"/>
+      <c r="B27" s="45"/>
       <c r="E27" s="6"/>
       <c r="F27" s="39"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="41"/>
+    <row r="28" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A28" s="46"/>
+      <c r="B28" s="45"/>
       <c r="E28" s="6"/>
       <c r="F28" s="39"/>
     </row>
@@ -6955,515 +6165,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383EB36A-4258-4DB9-A935-1380973574F9}">
-  <dimension ref="A1:G31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="C1" s="55" t="str">
-        <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
-        <v>Save As Converting_test_cases.xlsx</v>
-      </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-    </row>
-    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1234.123</v>
-      </c>
-      <c r="D12" s="7">
-        <v>1234.123</v>
-      </c>
-      <c r="E12" s="57" t="s">
-        <v>128</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="F15" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E17" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="F17" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
-      <c r="B18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="39"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="39"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
-      <c r="B20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="39"/>
-    </row>
-    <row r="21" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="41"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="39"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="41"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="39"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="41"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="39"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="41"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="39"/>
-    </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="41"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="39"/>
-    </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="41"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="39"/>
-    </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
-      <c r="B29" s="41"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="39"/>
-    </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="41"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="39"/>
-    </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="41"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="39"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="C1:G1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="F4:F1048576">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>ISNUMBER(SEARCH("PASS",$F4))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>ISNUMBER(SEARCH("FAIL",$F4))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7AA91D-298A-428D-991E-0B5E00F15C05}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -7471,49 +6172,49 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.40625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="55" t="str">
+      <c r="C1" s="50" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As manipulating_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-    </row>
-    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+    </row>
+    <row r="2" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="43" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="47" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -7532,11 +6233,11 @@
       <c r="F3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
@@ -7559,7 +6260,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A5" s="16" t="s">
         <v>28</v>
       </c>
@@ -7582,7 +6283,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="117" x14ac:dyDescent="0.6">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -7605,48 +6306,48 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A7" s="34"/>
       <c r="B7" s="33"/>
       <c r="C7" s="34"/>
       <c r="E7" s="34"/>
       <c r="F7" s="39"/>
-      <c r="G7" s="50"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="G7" s="55"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A8" s="34"/>
       <c r="B8" s="33"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
       <c r="F8" s="39"/>
-      <c r="G8" s="44"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="48"/>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A9" s="34"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="44"/>
-    </row>
-    <row r="10" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51" t="s">
+      <c r="G9" s="48"/>
+    </row>
+    <row r="10" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A10" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="43" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="47" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A11" s="26" t="s">
         <v>4</v>
       </c>
@@ -7669,7 +6370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A12" s="16" t="s">
         <v>28</v>
       </c>
@@ -7679,7 +6380,7 @@
       <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="53" t="s">
         <v>98</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -7692,7 +6393,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A13" s="16" t="s">
         <v>28</v>
       </c>
@@ -7702,7 +6403,7 @@
       <c r="C13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="53" t="s">
         <v>100</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -7715,7 +6416,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="237.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="234" x14ac:dyDescent="0.6">
       <c r="A14" s="16" t="s">
         <v>28</v>
       </c>
@@ -7738,7 +6439,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="65" x14ac:dyDescent="0.6">
       <c r="A15" s="16" t="s">
         <v>28</v>
       </c>
@@ -7749,7 +6450,7 @@
         <v>103</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="49" t="s">
+      <c r="E15" s="54" t="s">
         <v>100</v>
       </c>
       <c r="F15" s="17" t="s">
@@ -7757,7 +6458,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="119.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="117.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A16" s="16" t="s">
         <v>28</v>
       </c>
@@ -7780,22 +6481,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51" t="s">
+    <row r="17" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A17" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="43" t="s">
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="47" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A18" s="26" t="s">
         <v>4</v>
       </c>
@@ -7818,57 +6519,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="41"/>
+    <row r="19" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A19" s="46"/>
+      <c r="B19" s="45"/>
       <c r="E19" s="6"/>
       <c r="F19" s="39"/>
     </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
-      <c r="B20" s="41"/>
+    <row r="20" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A20" s="46"/>
+      <c r="B20" s="45"/>
       <c r="E20" s="6"/>
       <c r="F20" s="39"/>
     </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="41"/>
+    <row r="21" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A21" s="46"/>
+      <c r="B21" s="45"/>
       <c r="E21" s="6"/>
       <c r="F21" s="39"/>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="41"/>
+    <row r="22" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A22" s="46"/>
+      <c r="B22" s="45"/>
       <c r="E22" s="6"/>
       <c r="F22" s="39"/>
     </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="41"/>
+    <row r="23" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A23" s="46"/>
+      <c r="B23" s="45"/>
       <c r="E23" s="6"/>
       <c r="F23" s="39"/>
     </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="41"/>
+    <row r="24" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A24" s="46"/>
+      <c r="B24" s="45"/>
       <c r="E24" s="6"/>
       <c r="F24" s="39"/>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="41"/>
+    <row r="25" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A25" s="46"/>
+      <c r="B25" s="45"/>
       <c r="E25" s="6"/>
       <c r="F25" s="39"/>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="41"/>
+    <row r="26" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A26" s="46"/>
+      <c r="B26" s="45"/>
       <c r="E26" s="6"/>
       <c r="F26" s="39"/>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="41"/>
+    <row r="27" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A27" s="46"/>
+      <c r="B27" s="45"/>
       <c r="E27" s="6"/>
       <c r="F27" s="39"/>
     </row>
@@ -7893,7 +6594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0226E82-A952-4DAE-99A1-1227AB972715}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -7901,49 +6602,49 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.40625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="55" t="str">
+      <c r="C1" s="50" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As fundamentals_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-    </row>
-    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+    </row>
+    <row r="2" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="43" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="47" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -7962,11 +6663,11 @@
       <c r="F3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A4" s="16" t="s">
         <v>37</v>
       </c>
@@ -7989,7 +6690,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A5" s="16" t="s">
         <v>37</v>
       </c>
@@ -8012,7 +6713,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="52" x14ac:dyDescent="0.6">
       <c r="A6" s="16" t="s">
         <v>37</v>
       </c>
@@ -8035,7 +6736,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="39" x14ac:dyDescent="0.6">
       <c r="A7" s="16" t="s">
         <v>37</v>
       </c>
@@ -8056,7 +6757,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="39" x14ac:dyDescent="0.6">
       <c r="A8" s="16" t="s">
         <v>37</v>
       </c>
@@ -8079,31 +6780,31 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A9" s="34"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="44"/>
-    </row>
-    <row r="10" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51" t="s">
+      <c r="G9" s="48"/>
+    </row>
+    <row r="10" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A10" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="43" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="47" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A11" s="26" t="s">
         <v>4</v>
       </c>
@@ -8126,7 +6827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -8147,7 +6848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
       <c r="A13" s="16" t="s">
         <v>37</v>
       </c>
@@ -8168,7 +6869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="65" x14ac:dyDescent="0.6">
       <c r="A14" s="16" t="s">
         <v>37</v>
       </c>
@@ -8189,7 +6890,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="39" x14ac:dyDescent="0.6">
       <c r="A15" s="16" t="s">
         <v>37</v>
       </c>
@@ -8210,34 +6911,34 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
-      <c r="B16" s="41"/>
+    <row r="16" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A16" s="46"/>
+      <c r="B16" s="45"/>
       <c r="E16" s="6"/>
       <c r="F16" s="39"/>
     </row>
-    <row r="17" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
-      <c r="B17" s="41"/>
+    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A17" s="46"/>
+      <c r="B17" s="45"/>
       <c r="E17" s="6"/>
       <c r="F17" s="39"/>
     </row>
-    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51" t="s">
+    <row r="18" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A18" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="43" t="s">
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="47" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A19" s="26" t="s">
         <v>4</v>
       </c>
@@ -8260,57 +6961,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
-      <c r="B20" s="41"/>
+    <row r="20" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A20" s="46"/>
+      <c r="B20" s="45"/>
       <c r="E20" s="6"/>
       <c r="F20" s="39"/>
     </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="41"/>
+    <row r="21" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A21" s="46"/>
+      <c r="B21" s="45"/>
       <c r="E21" s="6"/>
       <c r="F21" s="39"/>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="41"/>
+    <row r="22" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A22" s="46"/>
+      <c r="B22" s="45"/>
       <c r="E22" s="6"/>
       <c r="F22" s="39"/>
     </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="41"/>
+    <row r="23" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A23" s="46"/>
+      <c r="B23" s="45"/>
       <c r="E23" s="6"/>
       <c r="F23" s="39"/>
     </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="41"/>
+    <row r="24" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A24" s="46"/>
+      <c r="B24" s="45"/>
       <c r="E24" s="6"/>
       <c r="F24" s="39"/>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="41"/>
+    <row r="25" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A25" s="46"/>
+      <c r="B25" s="45"/>
       <c r="E25" s="6"/>
       <c r="F25" s="39"/>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="41"/>
+    <row r="26" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A26" s="46"/>
+      <c r="B26" s="45"/>
       <c r="E26" s="6"/>
       <c r="F26" s="39"/>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="41"/>
+    <row r="27" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A27" s="46"/>
+      <c r="B27" s="45"/>
       <c r="E27" s="6"/>
       <c r="F27" s="39"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="41"/>
+    <row r="28" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="A28" s="46"/>
+      <c r="B28" s="45"/>
       <c r="E28" s="6"/>
       <c r="F28" s="39"/>
     </row>
@@ -8335,18 +7036,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DE6347-7E0A-47D6-BA4D-B2ACFD9544D5}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="AER1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="89.5546875" customWidth="1"/>
+    <col min="1" max="1" width="89.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="24" t="s">
         <v>74</v>
       </c>
@@ -8524,6 +7225,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="834b100a-dc26-4ede-9885-7b3df77c2ec4">
@@ -8531,15 +7241,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8561,6 +7262,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDA4F701-CB39-492A-9F08-5608EAF6F285}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77858E8B-8BDD-41DD-927E-8B417020F918}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8568,12 +7277,4 @@
     <ds:schemaRef ds:uri="834b100a-dc26-4ede-9885-7b3df77c2ec4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDA4F701-CB39-492A-9F08-5608EAF6F285}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added submitted Final-Test-Cases.xslx for version2
</commit_message>
<xml_diff>
--- a/3Final-Project-Test-Cases.xlsx
+++ b/3Final-Project-Test-Cases.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cpr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca-my.sharepoint.com/personal/ldang15_myseneca_ca/Documents/CPRZII/w11_final_project_planning/to_submit_version_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56B7D08-474C-4E75-8674-4E4BE9447635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F56B7D08-474C-4E75-8674-4E4BE9447635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5D1BBC0-9FD7-4914-9C82-13735BE25256}"/>
   <bookViews>
-    <workbookView xWindow="9525" yWindow="0" windowWidth="9750" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
     <sheet name="fundamentals" sheetId="9" r:id="rId2"/>
-    <sheet name="manipulating" sheetId="10" r:id="rId3"/>
-    <sheet name="tokenizing" sheetId="11" r:id="rId4"/>
-    <sheet name="click-drag add module test here" sheetId="8" r:id="rId5"/>
+    <sheet name="converting" sheetId="12" r:id="rId3"/>
+    <sheet name="manipulating" sheetId="10" r:id="rId4"/>
+    <sheet name="tokenizing" sheetId="11" r:id="rId5"/>
+    <sheet name="click-drag add module test here" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1985,7 +1986,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
       <text>
         <r>
           <rPr>
@@ -2029,7 +2030,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
       <text>
         <r>
           <rPr>
@@ -2094,7 +2095,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
       <text>
         <r>
           <rPr>
@@ -2120,7 +2121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
       <text>
         <r>
           <rPr>
@@ -2165,7 +2166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
       <text>
         <r>
           <rPr>
@@ -2189,7 +2190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
       <text>
         <r>
           <rPr>
@@ -2212,7 +2213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
       <text>
         <r>
           <rPr>
@@ -2232,6 +2233,742 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tim McKenna</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{73CDDCC5-DEF9-4198-AB6F-663FBFA75AEC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+general description of a test.
+Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{C5E57DF2-75BE-427E-B461-846D7F195E14}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
++</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{4679AE41-C1FC-42AC-AC68-EBAC777A24D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Test Input:
+exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is similar to source code in a program: it describes exactly how it will be done.
+The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{2891D1DC-16FD-429F-AADE-260368988D34}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output or Response:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+the result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the test is run.
+This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{56C701D0-649D-415A-8827-D8C01E5844B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hover over Result and Comments for more details.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{1CFD9AEA-4F24-48EF-8683-675BA2D08F3F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Result:
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{7AB124D7-8C8A-44DD-A61F-3B2C3D2DE3F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Required for negative test cases that FAIL
+or for unexpect results.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{F73B17DE-5D6D-4BEE-8A16-22F591181658}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+general description of a test.
+Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{F368EADF-F05B-4C15-A4E0-CA9F2F783275}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
++</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{89399E78-2781-46CB-8982-30E3233EC7BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Test Input:
+exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is similar to source code in a program: it describes exactly how it will be done.
+The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{34FB52D3-7A1D-4C5B-9838-1E77E035A0FA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output or Response:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+the result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the test is run.
+This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{400DA026-3EB6-4927-87CA-8598E92E8996}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hover over Result and Comments for more details.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{9E419422-AFBA-4A9D-AF8D-AF50B3D1D5D0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Result:
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{99451D2F-B00E-4B10-92E4-565F887D03DF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Required for negative test cases that FAIL
+or for unexpect results.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+general description of a test.
+Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
++</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Test Input:
+exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is similar to source code in a program: it describes exactly how it will be done.
+The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output or Response:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+the result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the test is run.
+This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hover over Result and Comments for more details.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Result:
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Required for negative test cases that FAIL
+or for unexpect results.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tim McKenna</author>
@@ -2990,7 +3727,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="130">
   <si>
     <t>Program
 or module:</t>
@@ -3482,6 +4219,39 @@
   </si>
   <si>
     <t>,,,,,,,,,,</t>
+  </si>
+  <si>
+    <t>0.000000</t>
+  </si>
+  <si>
+    <t>a warning</t>
+  </si>
+  <si>
+    <t>- unexpected input</t>
+  </si>
+  <si>
+    <t>zasd~</t>
+  </si>
+  <si>
+    <t>The program does not handle strings longer than 16 char correctly</t>
+  </si>
+  <si>
+    <t>11111111111111112.000000</t>
+  </si>
+  <si>
+    <t>11111111111111111</t>
+  </si>
+  <si>
+    <t>- neagetive edge case</t>
+  </si>
+  <si>
+    <t>+ maximum edge case</t>
+  </si>
+  <si>
+    <t>1234.123000</t>
+  </si>
+  <si>
+    <t>Converting</t>
   </si>
 </sst>
 </file>
@@ -3949,7 +4719,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4069,18 +4839,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4095,9 +4853,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4114,12 +4869,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB4B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB4E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4504,22 +5294,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="88" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="88" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.31640625" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.453125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.31640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.31640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.6796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -4527,22 +5317,22 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>main</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="41" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="30" t="s">
         <v>3</v>
       </c>
@@ -4550,7 +5340,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -4574,7 +5364,7 @@
       </c>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>11</v>
       </c>
@@ -4601,7 +5391,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
@@ -4626,7 +5416,7 @@
       <c r="H5" s="25"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="143" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
@@ -4651,7 +5441,7 @@
       <c r="H6" s="25"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="65" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
@@ -4676,7 +5466,7 @@
       <c r="H7" s="25"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
@@ -4704,7 +5494,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="117" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>28</v>
       </c>
@@ -4732,7 +5522,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="117" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>28</v>
       </c>
@@ -4760,7 +5550,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="117" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>28</v>
       </c>
@@ -4788,7 +5578,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -4816,7 +5606,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>37</v>
       </c>
@@ -4844,7 +5634,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="52" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>37</v>
       </c>
@@ -4872,7 +5662,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="39" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>37</v>
       </c>
@@ -4894,7 +5684,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="39" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>37</v>
       </c>
@@ -4918,7 +5708,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>50</v>
       </c>
@@ -4942,7 +5732,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>50</v>
       </c>
@@ -4970,7 +5760,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>50</v>
       </c>
@@ -4998,7 +5788,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="68.900000000000006" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>50</v>
       </c>
@@ -5026,7 +5816,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="68.900000000000006" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>50</v>
       </c>
@@ -5050,7 +5840,7 @@
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="68.900000000000006" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:9" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>50</v>
       </c>
@@ -5074,7 +5864,7 @@
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="68.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+    <row r="23" spans="1:9" ht="68.849999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="s">
         <v>50</v>
       </c>
@@ -5098,14 +5888,14 @@
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A24" s="41" t="s">
+    <row r="24" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
       <c r="F24" s="30" t="s">
         <v>3</v>
       </c>
@@ -5113,7 +5903,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
         <v>4</v>
       </c>
@@ -5136,7 +5926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>11</v>
       </c>
@@ -5160,7 +5950,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>11</v>
       </c>
@@ -5184,7 +5974,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>11</v>
       </c>
@@ -5208,7 +5998,7 @@
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>28</v>
       </c>
@@ -5218,7 +6008,7 @@
       <c r="C29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="53" t="s">
+      <c r="D29" s="48" t="s">
         <v>98</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -5232,7 +6022,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>28</v>
       </c>
@@ -5242,7 +6032,7 @@
       <c r="C30" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="53" t="s">
+      <c r="D30" s="48" t="s">
         <v>100</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -5256,7 +6046,7 @@
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="234" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>28</v>
       </c>
@@ -5280,7 +6070,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="65" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>28</v>
       </c>
@@ -5291,7 +6081,7 @@
         <v>103</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="E32" s="54" t="s">
+      <c r="E32" s="49" t="s">
         <v>100</v>
       </c>
       <c r="F32" s="17" t="s">
@@ -5300,7 +6090,7 @@
       <c r="G32" s="3"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="117" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>28</v>
       </c>
@@ -5324,7 +6114,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>37</v>
       </c>
@@ -5346,7 +6136,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>37</v>
       </c>
@@ -5368,7 +6158,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="65" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>37</v>
       </c>
@@ -5390,7 +6180,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="39" x14ac:dyDescent="0.65">
+    <row r="37" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>37</v>
       </c>
@@ -5412,7 +6202,7 @@
       </c>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" ht="15.25" x14ac:dyDescent="0.65">
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>50</v>
       </c>
@@ -5431,7 +6221,7 @@
       </c>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>50</v>
       </c>
@@ -5455,7 +6245,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
         <v>50</v>
       </c>
@@ -5474,14 +6264,14 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A41" s="41" t="s">
+    <row r="41" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
       <c r="F41" s="30" t="s">
         <v>3</v>
       </c>
@@ -5489,7 +6279,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
         <v>4</v>
       </c>
@@ -5512,7 +6302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>11</v>
       </c>
@@ -5526,7 +6316,7 @@
       <c r="G43" s="3"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>11</v>
       </c>
@@ -5540,7 +6330,7 @@
       <c r="G44" s="3"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>11</v>
       </c>
@@ -5554,7 +6344,7 @@
       <c r="G45" s="3"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>28</v>
       </c>
@@ -5568,7 +6358,7 @@
       <c r="G46" s="3"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>28</v>
       </c>
@@ -5582,7 +6372,7 @@
       <c r="G47" s="3"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>28</v>
       </c>
@@ -5596,7 +6386,7 @@
       <c r="G48" s="3"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>37</v>
       </c>
@@ -5610,7 +6400,7 @@
       <c r="G49" s="3"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>37</v>
       </c>
@@ -5624,7 +6414,7 @@
       <c r="G50" s="3"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>37</v>
       </c>
@@ -5638,7 +6428,7 @@
       <c r="G51" s="3"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>50</v>
       </c>
@@ -5652,7 +6442,7 @@
       <c r="G52" s="3"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>50</v>
       </c>
@@ -5666,7 +6456,7 @@
       <c r="G53" s="3"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
         <v>50</v>
       </c>
@@ -5686,36 +6476,36 @@
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="F9:F11">
+    <cfRule type="expression" dxfId="15" priority="3">
+      <formula>ISNUMBER(SEARCH("PASS",$F9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="4">
+      <formula>ISNUMBER(SEARCH("FAIL",$F9))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29:F33">
+    <cfRule type="expression" dxfId="13" priority="1">
+      <formula>ISNUMBER(SEARCH("PASS",$F29))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="2">
+      <formula>ISNUMBER(SEARCH("FAIL",$F29))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F38">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>ISNUMBER(SEARCH("PASS",$F38))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>ISNUMBER(SEARCH("FAIL",$F38))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>ISNUMBER(SEARCH("PASS",$F40))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>ISNUMBER(SEARCH("FAIL",$F40))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9:F11">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>ISNUMBER(SEARCH("PASS",$F9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>ISNUMBER(SEARCH("FAIL",$F9))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F29:F33">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>ISNUMBER(SEARCH("PASS",$F29))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>ISNUMBER(SEARCH("FAIL",$F29))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5732,49 +6522,49 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.40625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="50" t="str">
+      <c r="C1" s="57" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As fundamentals_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="41" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="47" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -5793,11 +6583,11 @@
       <c r="F3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>11</v>
       </c>
@@ -5818,7 +6608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
@@ -5839,7 +6629,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="143" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
@@ -5860,7 +6650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="65" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
@@ -5883,7 +6673,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
@@ -5904,31 +6694,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="48"/>
-    </row>
-    <row r="10" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="41" t="s">
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="47" t="s">
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>4</v>
       </c>
@@ -5951,7 +6741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
@@ -5972,7 +6762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -5995,7 +6785,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="208" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="211.2" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>11</v>
       </c>
@@ -6018,7 +6808,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>11</v>
       </c>
@@ -6039,34 +6829,34 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A16" s="46"/>
-      <c r="B16" s="45"/>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="42"/>
+      <c r="B16" s="41"/>
       <c r="E16" s="6"/>
       <c r="F16" s="39"/>
     </row>
-    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A17" s="46"/>
-      <c r="B17" s="45"/>
+    <row r="17" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42"/>
+      <c r="B17" s="41"/>
       <c r="E17" s="6"/>
       <c r="F17" s="39"/>
     </row>
-    <row r="18" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="47" t="s">
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
         <v>4</v>
       </c>
@@ -6089,57 +6879,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A20" s="46"/>
-      <c r="B20" s="45"/>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="41"/>
       <c r="E20" s="6"/>
       <c r="F20" s="39"/>
     </row>
-    <row r="21" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A21" s="46"/>
-      <c r="B21" s="45"/>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="41"/>
       <c r="E21" s="6"/>
       <c r="F21" s="39"/>
     </row>
-    <row r="22" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A22" s="46"/>
-      <c r="B22" s="45"/>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="41"/>
       <c r="E22" s="6"/>
       <c r="F22" s="39"/>
     </row>
-    <row r="23" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A23" s="46"/>
-      <c r="B23" s="45"/>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="41"/>
       <c r="E23" s="6"/>
       <c r="F23" s="39"/>
     </row>
-    <row r="24" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A24" s="46"/>
-      <c r="B24" s="45"/>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="41"/>
       <c r="E24" s="6"/>
       <c r="F24" s="39"/>
     </row>
-    <row r="25" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A25" s="46"/>
-      <c r="B25" s="45"/>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="41"/>
       <c r="E25" s="6"/>
       <c r="F25" s="39"/>
     </row>
-    <row r="26" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A26" s="46"/>
-      <c r="B26" s="45"/>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="41"/>
       <c r="E26" s="6"/>
       <c r="F26" s="39"/>
     </row>
-    <row r="27" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A27" s="46"/>
-      <c r="B27" s="45"/>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="41"/>
       <c r="E27" s="6"/>
       <c r="F27" s="39"/>
     </row>
-    <row r="28" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A28" s="46"/>
-      <c r="B28" s="45"/>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="41"/>
       <c r="E28" s="6"/>
       <c r="F28" s="39"/>
     </row>
@@ -6151,10 +6941,10 @@
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F9:F1048576">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>ISNUMBER(SEARCH("PASS",$F9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>ISNUMBER(SEARCH("FAIL",$F9))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6165,6 +6955,515 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383EB36A-4258-4DB9-A935-1380973574F9}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="57" t="str">
+        <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
+        <v>Save As Converting_test_cases.xlsx</v>
+      </c>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1234.123</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1234.123</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="42"/>
+      <c r="B18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="39"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="42"/>
+      <c r="B19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="39"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="42"/>
+      <c r="B20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="39"/>
+    </row>
+    <row r="21" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="41"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="39"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="41"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="39"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="41"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="39"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="41"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="39"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="41"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="39"/>
+    </row>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="41"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="39"/>
+    </row>
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="42"/>
+      <c r="B29" s="41"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="39"/>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="42"/>
+      <c r="B30" s="41"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="39"/>
+    </row>
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="42"/>
+      <c r="B31" s="41"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="C1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F4:F1048576">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>ISNUMBER(SEARCH("PASS",$F4))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>ISNUMBER(SEARCH("FAIL",$F4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7AA91D-298A-428D-991E-0B5E00F15C05}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -6172,49 +7471,49 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.40625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="50" t="str">
+      <c r="C1" s="57" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As manipulating_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="41" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="47" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -6233,11 +7532,11 @@
       <c r="F3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
@@ -6260,7 +7559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>28</v>
       </c>
@@ -6283,7 +7582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="117" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -6306,48 +7605,48 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="33"/>
       <c r="C7" s="34"/>
       <c r="E7" s="34"/>
       <c r="F7" s="39"/>
-      <c r="G7" s="55"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+      <c r="G7" s="50"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="33"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
       <c r="F8" s="39"/>
-      <c r="G8" s="48"/>
-    </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="G8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="48"/>
-    </row>
-    <row r="10" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="41" t="s">
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="47" t="s">
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>4</v>
       </c>
@@ -6370,7 +7669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>28</v>
       </c>
@@ -6380,7 +7679,7 @@
       <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="48" t="s">
         <v>98</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -6393,7 +7692,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>28</v>
       </c>
@@ -6403,7 +7702,7 @@
       <c r="C13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="48" t="s">
         <v>100</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -6416,7 +7715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="234" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>28</v>
       </c>
@@ -6439,7 +7738,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="65" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>28</v>
       </c>
@@ -6450,7 +7749,7 @@
         <v>103</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="49" t="s">
         <v>100</v>
       </c>
       <c r="F15" s="17" t="s">
@@ -6458,7 +7757,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="117.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:7" ht="119.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>28</v>
       </c>
@@ -6481,22 +7780,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="47" t="s">
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>4</v>
       </c>
@@ -6519,57 +7818,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A19" s="46"/>
-      <c r="B19" s="45"/>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="42"/>
+      <c r="B19" s="41"/>
       <c r="E19" s="6"/>
       <c r="F19" s="39"/>
     </row>
-    <row r="20" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A20" s="46"/>
-      <c r="B20" s="45"/>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="41"/>
       <c r="E20" s="6"/>
       <c r="F20" s="39"/>
     </row>
-    <row r="21" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A21" s="46"/>
-      <c r="B21" s="45"/>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="41"/>
       <c r="E21" s="6"/>
       <c r="F21" s="39"/>
     </row>
-    <row r="22" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A22" s="46"/>
-      <c r="B22" s="45"/>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="41"/>
       <c r="E22" s="6"/>
       <c r="F22" s="39"/>
     </row>
-    <row r="23" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A23" s="46"/>
-      <c r="B23" s="45"/>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="41"/>
       <c r="E23" s="6"/>
       <c r="F23" s="39"/>
     </row>
-    <row r="24" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A24" s="46"/>
-      <c r="B24" s="45"/>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="41"/>
       <c r="E24" s="6"/>
       <c r="F24" s="39"/>
     </row>
-    <row r="25" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A25" s="46"/>
-      <c r="B25" s="45"/>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="41"/>
       <c r="E25" s="6"/>
       <c r="F25" s="39"/>
     </row>
-    <row r="26" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A26" s="46"/>
-      <c r="B26" s="45"/>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="41"/>
       <c r="E26" s="6"/>
       <c r="F26" s="39"/>
     </row>
-    <row r="27" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A27" s="46"/>
-      <c r="B27" s="45"/>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="41"/>
       <c r="E27" s="6"/>
       <c r="F27" s="39"/>
     </row>
@@ -6594,7 +7893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0226E82-A952-4DAE-99A1-1227AB972715}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -6602,49 +7901,49 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.40625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="50" t="str">
+      <c r="C1" s="57" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As fundamentals_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="41" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="47" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -6663,11 +7962,11 @@
       <c r="F3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>37</v>
       </c>
@@ -6690,7 +7989,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>37</v>
       </c>
@@ -6713,7 +8012,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="52" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>37</v>
       </c>
@@ -6736,7 +8035,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="39" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>37</v>
       </c>
@@ -6757,7 +8056,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="39" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>37</v>
       </c>
@@ -6780,31 +8079,31 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="48"/>
-    </row>
-    <row r="10" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="41" t="s">
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="47" t="s">
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>4</v>
       </c>
@@ -6827,7 +8126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -6848,7 +8147,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>37</v>
       </c>
@@ -6869,7 +8168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="65" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>37</v>
       </c>
@@ -6890,7 +8189,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="39" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>37</v>
       </c>
@@ -6911,34 +8210,34 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A16" s="46"/>
-      <c r="B16" s="45"/>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="42"/>
+      <c r="B16" s="41"/>
       <c r="E16" s="6"/>
       <c r="F16" s="39"/>
     </row>
-    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A17" s="46"/>
-      <c r="B17" s="45"/>
+    <row r="17" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42"/>
+      <c r="B17" s="41"/>
       <c r="E17" s="6"/>
       <c r="F17" s="39"/>
     </row>
-    <row r="18" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="47" t="s">
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="43" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="26.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
         <v>4</v>
       </c>
@@ -6961,57 +8260,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A20" s="46"/>
-      <c r="B20" s="45"/>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="41"/>
       <c r="E20" s="6"/>
       <c r="F20" s="39"/>
     </row>
-    <row r="21" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A21" s="46"/>
-      <c r="B21" s="45"/>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="41"/>
       <c r="E21" s="6"/>
       <c r="F21" s="39"/>
     </row>
-    <row r="22" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A22" s="46"/>
-      <c r="B22" s="45"/>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="41"/>
       <c r="E22" s="6"/>
       <c r="F22" s="39"/>
     </row>
-    <row r="23" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A23" s="46"/>
-      <c r="B23" s="45"/>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="41"/>
       <c r="E23" s="6"/>
       <c r="F23" s="39"/>
     </row>
-    <row r="24" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A24" s="46"/>
-      <c r="B24" s="45"/>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="41"/>
       <c r="E24" s="6"/>
       <c r="F24" s="39"/>
     </row>
-    <row r="25" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A25" s="46"/>
-      <c r="B25" s="45"/>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="41"/>
       <c r="E25" s="6"/>
       <c r="F25" s="39"/>
     </row>
-    <row r="26" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A26" s="46"/>
-      <c r="B26" s="45"/>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="41"/>
       <c r="E26" s="6"/>
       <c r="F26" s="39"/>
     </row>
-    <row r="27" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A27" s="46"/>
-      <c r="B27" s="45"/>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="41"/>
       <c r="E27" s="6"/>
       <c r="F27" s="39"/>
     </row>
-    <row r="28" spans="1:7" ht="15.25" x14ac:dyDescent="0.6">
-      <c r="A28" s="46"/>
-      <c r="B28" s="45"/>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="41"/>
       <c r="E28" s="6"/>
       <c r="F28" s="39"/>
     </row>
@@ -7036,18 +8335,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DE6347-7E0A-47D6-BA4D-B2ACFD9544D5}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="AER1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.54296875" customWidth="1"/>
+    <col min="1" max="1" width="89.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>74</v>
       </c>

</xml_diff>